<commit_message>
Jar info moved to parts list
</commit_message>
<xml_diff>
--- a/JacobLadderPL.xlsx
+++ b/JacobLadderPL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\JacobsLadder\Parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\JacobsLadder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEB4B24-57BF-43B4-9B68-59DFE5655071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35D2DF1-3A7D-4761-9B86-FAE9B9119EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1824" yWindow="2232" windowWidth="17232" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Jacob's Ladder Parts List</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>ModuleLive</t>
+  </si>
+  <si>
+    <t>2.04" (52 mm)</t>
+  </si>
+  <si>
+    <t>2.32" (59 mm)</t>
+  </si>
+  <si>
+    <t>Jar Description</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jar Inner Opening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jar Outer Opening </t>
   </si>
 </sst>
 </file>
@@ -222,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -277,6 +295,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -558,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,6 +787,33 @@
         <v>58.59</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>